<commit_message>
adding br-003, br-004, br-005, br-006
</commit_message>
<xml_diff>
--- a/tests/manual/test-cases.xlsx
+++ b/tests/manual/test-cases.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\art\tests\manual\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\pa\art\tests\manual\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CAE5237-136B-47C4-BD1F-02FFDE347249}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -24,10 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="53">
-  <si>
-    <t>Модуль</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="60">
   <si>
     <t>Предусловия</t>
   </si>
@@ -47,15 +45,9 @@
     <t>Заголовок</t>
   </si>
   <si>
-    <t>Открыта страница МШК-04</t>
-  </si>
-  <si>
     <t>Произошел переход на страницу МШК-01</t>
   </si>
   <si>
-    <t>Шапка сайта</t>
-  </si>
-  <si>
     <t>1. Нажать ЛКМ на логотип в шапке сайта</t>
   </si>
   <si>
@@ -69,9 +61,6 @@
   </si>
   <si>
     <t>Произошел переход в начало страницы</t>
-  </si>
-  <si>
-    <t>Произошел переход на страницу МШК-04</t>
   </si>
   <si>
     <t>Произошел переход на страницу МШК-06</t>
@@ -105,11 +94,6 @@
   <si>
     <t>1. Нажать ЛКМ на пункт "МШК-04" в панели
 главного меню</t>
-  </si>
-  <si>
-    <t>А. Открыта главная страница
-Б. Установлена ширина экрана
-768 px</t>
   </si>
   <si>
     <t>2. Нажать ЛКМ на значек закрытия главного
@@ -127,12 +111,6 @@
   <si>
     <t>Проверка работы ссылок главного
 меню при ширине экрана 320 px</t>
-  </si>
-  <si>
-    <t>Проверка условия №1</t>
-  </si>
-  <si>
-    <t>Конфигуратор МШК-01</t>
   </si>
   <si>
     <t>1. Для параметра "Отдельно стоящий"
@@ -149,9 +127,6 @@
 значение "550", погашен.</t>
   </si>
   <si>
-    <t>Кнопка Скачать Excel</t>
-  </si>
-  <si>
     <t>Проверка работы
 кнопки "Скачать Excel"</t>
   </si>
@@ -161,9 +136,6 @@
   </si>
   <si>
     <t>Браузер загрузил файл</t>
-  </si>
-  <si>
-    <t>Проверка условия №2</t>
   </si>
   <si>
     <t>1. Для параметра "Отдельно стоящий"
@@ -209,9 +181,6 @@
 Г. Таблица раздельной выписки и
 кнопка "Скачать Excel" скрыты.</t>
     </r>
-  </si>
-  <si>
-    <t>Проверка условия №3</t>
   </si>
   <si>
     <t>1. Для параметра "Механизм дивана"
@@ -272,11 +241,68 @@
     <t>А. Страница МШК-01 перезагружена
 Б. Работа с конфигуратором МШК-01</t>
   </si>
+  <si>
+    <t>Требование</t>
+  </si>
+  <si>
+    <t>4.2.1.2</t>
+  </si>
+  <si>
+    <t>failed</t>
+  </si>
+  <si>
+    <t>passed</t>
+  </si>
+  <si>
+    <t>А. Открыта главная страница
+Б. Установлена ширина экрана
+768 px
+В. В панели главного меню подчеркнут пункт "МШК-01"</t>
+  </si>
+  <si>
+    <t>1. Произошел переход на страницу
+МШК-04
+2. В панели главного меню подчеркнут пункт "МШК-04"</t>
+  </si>
+  <si>
+    <t>4.2.3.4</t>
+  </si>
+  <si>
+    <t>4.2.1.5</t>
+  </si>
+  <si>
+    <t>4.2.1.3</t>
+  </si>
+  <si>
+    <t>4.2.1.10</t>
+  </si>
+  <si>
+    <t>4.2.2.4
+4.2.3.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 4.4.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 4.4.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 4.4.3</t>
+  </si>
+  <si>
+    <t>Проверка требования 4.4.1</t>
+  </si>
+  <si>
+    <t>Проверка требования 4.4.2</t>
+  </si>
+  <si>
+    <t>Проверка требования 4.4.3</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -303,7 +329,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -316,6 +342,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="24">
     <border>
@@ -642,7 +680,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -661,7 +699,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -680,15 +717,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -707,80 +738,131 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1096,19 +1178,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F14" sqref="F14"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="7.5546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="23.33203125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="34.88671875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="23.33203125" style="61" customWidth="1"/>
+    <col min="3" max="3" width="37.88671875" style="1" customWidth="1"/>
     <col min="4" max="4" width="39.21875" style="1" customWidth="1"/>
     <col min="5" max="5" width="43.6640625" style="1" customWidth="1"/>
     <col min="6" max="6" width="42.6640625" style="1" customWidth="1"/>
@@ -1118,306 +1200,326 @@
   <sheetData>
     <row r="1" spans="1:7" s="2" customFormat="1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="49" t="s">
+        <v>43</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="6" t="s">
         <v>4</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" s="6" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="7">
         <v>1</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="50" t="s">
+        <v>44</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="47" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="32">
+        <v>2</v>
+      </c>
+      <c r="B3" s="51" t="s">
+        <v>51</v>
+      </c>
+      <c r="C3" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="D3" s="34" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" s="44" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" s="33"/>
+      <c r="B4" s="52"/>
+      <c r="C4" s="35"/>
+      <c r="D4" s="35"/>
+      <c r="E4" s="38" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" s="39" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="G4" s="45"/>
+    </row>
+    <row r="5" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="41"/>
+      <c r="B5" s="53"/>
+      <c r="C5" s="42"/>
+      <c r="D5" s="42"/>
+      <c r="E5" s="42"/>
+      <c r="F5" s="42"/>
+      <c r="G5" s="46"/>
+    </row>
+    <row r="6" spans="1:7" s="12" customFormat="1" ht="71.400000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="13">
+        <v>3</v>
+      </c>
+      <c r="B6" s="50" t="s">
+        <v>50</v>
+      </c>
+      <c r="C6" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="E6" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="F6" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="G6" s="48" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" s="12" customFormat="1" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="32">
+        <v>4</v>
+      </c>
+      <c r="B7" s="54" t="s">
+        <v>53</v>
+      </c>
+      <c r="C7" s="36" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" s="36" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="F7" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="G7" s="44" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" s="12" customFormat="1" ht="29.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="41"/>
+      <c r="B8" s="53"/>
+      <c r="C8" s="43"/>
+      <c r="D8" s="43"/>
+      <c r="E8" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="F8" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="G8" s="46"/>
+    </row>
+    <row r="9" spans="1:7" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="32">
+        <v>5</v>
+      </c>
+      <c r="B9" s="51" t="s">
+        <v>49</v>
+      </c>
+      <c r="C9" s="36" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" s="36" t="s">
+        <v>24</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="F9" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="G9" s="44" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="25.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="33"/>
+      <c r="B10" s="52"/>
+      <c r="C10" s="37"/>
+      <c r="D10" s="37"/>
+      <c r="E10" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G10" s="45"/>
+    </row>
+    <row r="11" spans="1:7" ht="31.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="13">
+        <v>6</v>
+      </c>
+      <c r="B11" s="50" t="s">
+        <v>52</v>
+      </c>
+      <c r="C11" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="D11" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="E11" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="F11" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="G11" s="48" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" s="12" customFormat="1" ht="65.400000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="18">
         <v>7</v>
       </c>
-      <c r="E2" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" s="8" t="s">
+      <c r="B12" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="C12" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="D12" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="E12" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="F12" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="G12" s="63" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" s="12" customFormat="1" ht="37.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="23">
         <v>8</v>
       </c>
-      <c r="G2" s="10"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="31">
-        <v>2</v>
-      </c>
-      <c r="B3" s="33" t="s">
+      <c r="B13" s="55" t="s">
+        <v>55</v>
+      </c>
+      <c r="C13" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="D13" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="E13" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="F13" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="G13" s="64" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="142.19999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="40"/>
+      <c r="B14" s="56"/>
+      <c r="C14" s="39"/>
+      <c r="D14" s="38"/>
+      <c r="E14" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="F14" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="G14" s="65" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A15" s="23">
         <v>9</v>
       </c>
-      <c r="C3" s="33" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" s="33" t="s">
-        <v>18</v>
-      </c>
-      <c r="E3" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="F3" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="G3" s="28"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="39"/>
-      <c r="B4" s="40"/>
-      <c r="C4" s="40"/>
-      <c r="D4" s="40"/>
-      <c r="E4" s="38" t="s">
-        <v>22</v>
-      </c>
-      <c r="F4" s="37" t="s">
-        <v>14</v>
-      </c>
-      <c r="G4" s="29"/>
-    </row>
-    <row r="5" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="32"/>
-      <c r="B5" s="34"/>
-      <c r="C5" s="34"/>
-      <c r="D5" s="34"/>
-      <c r="E5" s="34"/>
-      <c r="F5" s="34"/>
-      <c r="G5" s="30"/>
-    </row>
-    <row r="6" spans="1:7" s="13" customFormat="1" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="14">
-        <v>3</v>
-      </c>
-      <c r="B6" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="D6" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="E6" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="F6" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="G6" s="17"/>
-    </row>
-    <row r="7" spans="1:7" s="13" customFormat="1" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="31">
-        <v>4</v>
-      </c>
-      <c r="B7" s="33" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" s="35" t="s">
-        <v>28</v>
-      </c>
-      <c r="D7" s="35" t="s">
-        <v>29</v>
-      </c>
-      <c r="E7" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="F7" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="G7" s="28"/>
-    </row>
-    <row r="8" spans="1:7" s="13" customFormat="1" ht="29.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="32"/>
-      <c r="B8" s="34"/>
-      <c r="C8" s="36"/>
-      <c r="D8" s="36"/>
-      <c r="E8" s="18" t="s">
+      <c r="B15" s="55" t="s">
+        <v>56</v>
+      </c>
+      <c r="C15" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="D15" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="F8" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="G8" s="30"/>
-    </row>
-    <row r="9" spans="1:7" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="31">
-        <v>5</v>
-      </c>
-      <c r="B9" s="33" t="s">
-        <v>9</v>
-      </c>
-      <c r="C9" s="35" t="s">
-        <v>30</v>
-      </c>
-      <c r="D9" s="35" t="s">
-        <v>29</v>
-      </c>
-      <c r="E9" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="F9" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="G9" s="28"/>
-    </row>
-    <row r="10" spans="1:7" ht="25.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="39"/>
-      <c r="B10" s="40"/>
-      <c r="C10" s="41"/>
-      <c r="D10" s="41"/>
-      <c r="E10" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="G10" s="29"/>
-    </row>
-    <row r="11" spans="1:7" ht="31.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="14">
-        <v>6</v>
-      </c>
-      <c r="B11" s="15" t="s">
+      <c r="E15" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="C11" s="16" t="s">
+      <c r="F15" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="D11" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="E11" s="16" t="s">
+      <c r="G15" s="44" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="37.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="24"/>
+      <c r="B16" s="57"/>
+      <c r="C16" s="30"/>
+      <c r="D16" s="27"/>
+      <c r="E16" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="F11" s="15" t="s">
+      <c r="F16" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="G11" s="17"/>
-    </row>
-    <row r="12" spans="1:7" s="13" customFormat="1" ht="65.400000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="21">
-        <v>7</v>
-      </c>
-      <c r="B12" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="C12" s="22" t="s">
-        <v>31</v>
-      </c>
-      <c r="D12" s="20" t="s">
-        <v>52</v>
-      </c>
-      <c r="E12" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="F12" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="G12" s="19"/>
-    </row>
-    <row r="13" spans="1:7" s="13" customFormat="1" ht="37.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="44">
-        <v>8</v>
-      </c>
-      <c r="B13" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="C13" s="43" t="s">
+      <c r="G16" s="45"/>
+    </row>
+    <row r="17" spans="1:7" ht="172.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="25"/>
+      <c r="B17" s="58"/>
+      <c r="C17" s="31"/>
+      <c r="D17" s="28"/>
+      <c r="E17" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="D13" s="42" t="s">
-        <v>34</v>
-      </c>
-      <c r="E13" s="25" t="s">
+      <c r="F17" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="F13" s="25" t="s">
-        <v>42</v>
-      </c>
-      <c r="G13" s="26"/>
-    </row>
-    <row r="14" spans="1:7" ht="142.19999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="45"/>
-      <c r="B14" s="37"/>
-      <c r="C14" s="37"/>
-      <c r="D14" s="38"/>
-      <c r="E14" s="23" t="s">
-        <v>43</v>
-      </c>
-      <c r="F14" s="23" t="s">
-        <v>44</v>
-      </c>
-      <c r="G14" s="27"/>
-    </row>
-    <row r="15" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A15" s="44">
-        <v>9</v>
-      </c>
-      <c r="B15" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="C15" s="43" t="s">
-        <v>45</v>
-      </c>
-      <c r="D15" s="42" t="s">
-        <v>34</v>
-      </c>
-      <c r="E15" s="25" t="s">
-        <v>46</v>
-      </c>
-      <c r="F15" s="25" t="s">
-        <v>47</v>
-      </c>
-      <c r="G15" s="28"/>
-    </row>
-    <row r="16" spans="1:7" ht="37.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="50"/>
-      <c r="B16" s="48"/>
-      <c r="C16" s="48"/>
-      <c r="D16" s="46"/>
-      <c r="E16" s="24" t="s">
-        <v>48</v>
-      </c>
-      <c r="F16" s="24" t="s">
-        <v>49</v>
-      </c>
-      <c r="G16" s="29"/>
-    </row>
-    <row r="17" spans="1:7" ht="172.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="51"/>
-      <c r="B17" s="49"/>
-      <c r="C17" s="49"/>
-      <c r="D17" s="47"/>
-      <c r="E17" s="18" t="s">
-        <v>50</v>
-      </c>
-      <c r="F17" s="18" t="s">
-        <v>51</v>
-      </c>
-      <c r="G17" s="30"/>
+      <c r="G17" s="46"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="4"/>
-      <c r="B18" s="4"/>
+      <c r="B18" s="59"/>
       <c r="C18" s="4"/>
       <c r="D18" s="4"/>
       <c r="E18" s="4"/>
@@ -1426,7 +1528,7 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="3"/>
-      <c r="B19" s="3"/>
+      <c r="B19" s="60"/>
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
@@ -1435,7 +1537,7 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="3"/>
-      <c r="B20" s="3"/>
+      <c r="B20" s="60"/>
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
       <c r="E20" s="3"/>
@@ -1444,7 +1546,7 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="3"/>
-      <c r="B21" s="3"/>
+      <c r="B21" s="60"/>
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
       <c r="E21" s="3"/>
@@ -1453,7 +1555,7 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="3"/>
-      <c r="B22" s="3"/>
+      <c r="B22" s="60"/>
       <c r="C22" s="3"/>
       <c r="D22" s="3"/>
       <c r="E22" s="3"/>
@@ -1462,7 +1564,7 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="3"/>
-      <c r="B23" s="3"/>
+      <c r="B23" s="60"/>
       <c r="C23" s="3"/>
       <c r="D23" s="3"/>
       <c r="E23" s="3"/>
@@ -1471,7 +1573,7 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="3"/>
-      <c r="B24" s="3"/>
+      <c r="B24" s="60"/>
       <c r="C24" s="3"/>
       <c r="D24" s="3"/>
       <c r="E24" s="3"/>
@@ -1480,7 +1582,7 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="3"/>
-      <c r="B25" s="3"/>
+      <c r="B25" s="60"/>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
       <c r="E25" s="3"/>
@@ -1489,6 +1591,18 @@
     </row>
   </sheetData>
   <mergeCells count="26">
+    <mergeCell ref="G3:G5"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="F4:F5"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="B3:B5"/>
+    <mergeCell ref="C3:C5"/>
+    <mergeCell ref="D3:D5"/>
+    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="D7:D8"/>
     <mergeCell ref="A15:A17"/>
     <mergeCell ref="G9:G10"/>
     <mergeCell ref="G15:G17"/>
@@ -1503,20 +1617,11 @@
     <mergeCell ref="C13:C14"/>
     <mergeCell ref="B13:B14"/>
     <mergeCell ref="A13:A14"/>
-    <mergeCell ref="G3:G5"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="F4:F5"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="A3:A5"/>
-    <mergeCell ref="B3:B5"/>
-    <mergeCell ref="C3:C5"/>
-    <mergeCell ref="D3:D5"/>
-    <mergeCell ref="G7:G8"/>
-    <mergeCell ref="D7:D8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="B12" twoDigitTextYear="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>